<commit_message>
Update of LaTeX document.
TODO:

PSUDO code of worst case runtime in discussion.
Write more in the discussion
Read through the whole document and check for errors.

AND COMMIT TO FRONTER!!
</commit_message>
<xml_diff>
--- a/Lab3/report/resultat 2016-02-01.xlsx
+++ b/Lab3/report/resultat 2016-02-01.xlsx
@@ -564,6 +564,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:yVal>
             <c:numRef>
               <c:f>Blad1!$O$8:$O$55</c:f>
@@ -2345,8 +2359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="F8" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>